<commit_message>
Performance comparison fully complete
</commit_message>
<xml_diff>
--- a/Project Repport/Comparaison des performances.xlsx
+++ b/Project Repport/Comparaison des performances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\FractalSharp\Project Repport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B10C2E-E21A-421C-82CC-01F86577D400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DC699A-BC2B-4D73-825A-6BCB3AC8D4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
   <si>
     <t>Windows</t>
   </si>
@@ -82,6 +83,9 @@
   </si>
   <si>
     <t>∞</t>
+  </si>
+  <si>
+    <t>16000*9000 : -2 2 -1.125 1.125</t>
   </si>
 </sst>
 </file>
@@ -137,13 +141,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -429,811 +433,1077 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE15"/>
+  <dimension ref="A1:AH16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
-    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.88671875" style="2"/>
-    <col min="13" max="13" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="8.88671875" style="2"/>
-    <col min="18" max="18" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="8.88671875" style="2"/>
-    <col min="23" max="23" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="27" width="8.88671875" style="2"/>
-    <col min="28" max="28" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="63.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="8.88671875" style="1"/>
+    <col min="18" max="18" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="8.88671875" style="1"/>
+    <col min="23" max="23" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="8.88671875" style="1"/>
+    <col min="28" max="28" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="8.88671875" style="1"/>
+    <col min="33" max="33" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.5546875" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="R2" s="1" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="R2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="W2" s="1" t="s">
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="W2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AB2" s="1" t="s">
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AB2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AG2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH2" s="4"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="5"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="O3" s="5"/>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="T3" s="5"/>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="X3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="4" t="s">
+      <c r="Z3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AC3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="AD3" s="5"/>
-      <c r="AE3" s="4" t="s">
+      <c r="AE3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="AH3" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="O4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W4" s="3" t="s">
+      <c r="T4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="X4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AC4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AD4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE4" s="4" t="s">
+      <c r="AD4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C5" s="4" t="s">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>0.94</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>0.21</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="H5" s="4" t="s">
+      <c r="F5" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>0.67</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>0.08</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="M5" s="4" t="s">
+      <c r="K5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>3.26</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>0.67</v>
       </c>
-      <c r="P5" s="4"/>
-      <c r="R5" s="4" t="s">
+      <c r="P5" s="3">
+        <v>2.08</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="3">
         <v>2.3199999999999998</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="3">
         <v>0.22</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="W5" s="4" t="s">
+      <c r="U5" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="W5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X5" s="3">
         <v>34.54</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="3">
         <v>5.68</v>
       </c>
-      <c r="Z5" s="4"/>
-      <c r="AB5" s="4" t="s">
+      <c r="Z5" s="3">
+        <v>15.52</v>
+      </c>
+      <c r="AB5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AC5" s="4">
+      <c r="AC5" s="3">
         <v>22.77</v>
       </c>
-      <c r="AD5" s="4">
+      <c r="AD5" s="3">
         <v>1.65</v>
       </c>
-      <c r="AE5" s="4"/>
+      <c r="AE5" s="3">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>268.27</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C6" s="4">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>1.5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0.17</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="H6" s="4">
+      <c r="F6" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="H6" s="3">
         <v>2</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>1.37</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>0.12</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="M6" s="4">
+      <c r="K6" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="M6" s="3">
         <v>2</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>4.83</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>0.43</v>
       </c>
-      <c r="P6" s="4"/>
-      <c r="R6" s="4">
+      <c r="P6" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="R6" s="3">
         <v>2</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="3">
         <v>4.45</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="3">
         <v>0.22</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="W6" s="4">
+      <c r="U6" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="W6" s="3">
         <v>2</v>
       </c>
-      <c r="X6" s="4">
+      <c r="X6" s="3">
         <v>64.7</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y6" s="3">
         <v>3.2</v>
       </c>
-      <c r="Z6" s="4"/>
-      <c r="AB6" s="4">
+      <c r="Z6" s="3">
+        <v>8.52</v>
+      </c>
+      <c r="AB6" s="3">
         <v>2</v>
       </c>
-      <c r="AC6" s="4">
+      <c r="AC6" s="3">
         <v>42.34</v>
       </c>
-      <c r="AD6" s="4">
+      <c r="AD6" s="3">
         <v>1.23</v>
       </c>
-      <c r="AE6" s="4"/>
+      <c r="AE6" s="3">
+        <v>3.33</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>133.82</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C7" s="4">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
         <v>1.74</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>0.2</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="H7" s="4">
-        <v>3</v>
-      </c>
-      <c r="I7" s="4">
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
         <v>1.53</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>0.15</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="M7" s="4">
-        <v>3</v>
-      </c>
-      <c r="N7" s="4">
+      <c r="K7" s="3">
+        <v>0.79</v>
+      </c>
+      <c r="M7" s="3">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3">
         <v>5.54</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>0.53</v>
       </c>
-      <c r="P7" s="4"/>
-      <c r="R7" s="4">
-        <v>3</v>
-      </c>
-      <c r="S7" s="4">
+      <c r="P7" s="3">
+        <v>1.91</v>
+      </c>
+      <c r="R7" s="3">
+        <v>3</v>
+      </c>
+      <c r="S7" s="3">
         <v>5.15</v>
       </c>
-      <c r="T7" s="4">
+      <c r="T7" s="3">
         <v>0.25</v>
       </c>
-      <c r="U7" s="4"/>
-      <c r="W7" s="4">
-        <v>3</v>
-      </c>
-      <c r="X7" s="4" t="s">
+      <c r="U7" s="3">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="W7" s="3">
+        <v>3</v>
+      </c>
+      <c r="X7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y7" s="3">
         <v>4.17</v>
       </c>
-      <c r="Z7" s="4"/>
-      <c r="AB7" s="4">
-        <v>3</v>
-      </c>
-      <c r="AC7" s="4" t="s">
+      <c r="Z7" s="3">
+        <v>10.92</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AD7" s="4">
+      <c r="AD7" s="3">
         <v>1.4</v>
       </c>
-      <c r="AE7" s="4"/>
+      <c r="AE7" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>206.36</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C8" s="4">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>1.87</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>0.18</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="H8" s="4">
+      <c r="F8" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="H8" s="3">
         <v>4</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>1.74</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K8" s="4"/>
-      <c r="M8" s="4">
+      <c r="K8" s="3">
+        <v>0.77</v>
+      </c>
+      <c r="M8" s="3">
         <v>4</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3">
         <v>6.34</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="3">
         <v>0.43</v>
       </c>
-      <c r="P8" s="4"/>
-      <c r="R8" s="4">
+      <c r="P8" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="R8" s="3">
         <v>4</v>
       </c>
-      <c r="S8" s="4">
+      <c r="S8" s="3">
         <v>5.57</v>
       </c>
-      <c r="T8" s="4">
+      <c r="T8" s="3">
         <v>0.23</v>
       </c>
-      <c r="U8" s="4"/>
-      <c r="W8" s="4">
+      <c r="U8" s="3">
+        <v>1.03</v>
+      </c>
+      <c r="W8" s="3">
         <v>4</v>
       </c>
-      <c r="X8" s="4">
+      <c r="X8" s="3">
         <v>71.72</v>
       </c>
-      <c r="Y8" s="4">
+      <c r="Y8" s="3">
         <v>2.93</v>
       </c>
-      <c r="Z8" s="4"/>
-      <c r="AB8" s="4">
+      <c r="Z8" s="3">
+        <v>7.61</v>
+      </c>
+      <c r="AB8" s="3">
         <v>4</v>
       </c>
-      <c r="AC8" s="4">
+      <c r="AC8" s="3">
         <v>55.79</v>
       </c>
-      <c r="AD8" s="4">
+      <c r="AD8" s="3">
         <v>1.1399999999999999</v>
       </c>
-      <c r="AE8" s="4"/>
+      <c r="AE8" s="3">
+        <v>3.05</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH8" s="3">
+        <v>119.22</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C9" s="4">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C9" s="3">
         <v>5</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>2.06</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>0.22</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="H9" s="4">
+      <c r="F9" s="3">
+        <v>0.86</v>
+      </c>
+      <c r="H9" s="3">
         <v>5</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>1.9</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>0.15</v>
       </c>
-      <c r="K9" s="4"/>
-      <c r="M9" s="4">
+      <c r="K9" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="M9" s="3">
         <v>5</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="3">
         <v>6.6</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="3">
         <v>0.44</v>
       </c>
-      <c r="P9" s="4"/>
-      <c r="R9" s="4">
+      <c r="P9" s="3">
+        <v>1.59</v>
+      </c>
+      <c r="R9" s="3">
         <v>5</v>
       </c>
-      <c r="S9" s="4">
+      <c r="S9" s="3">
         <v>6.14</v>
       </c>
-      <c r="T9" s="4">
+      <c r="T9" s="3">
         <v>0.24</v>
       </c>
-      <c r="U9" s="4"/>
-      <c r="W9" s="4">
+      <c r="U9" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="W9" s="3">
         <v>5</v>
       </c>
-      <c r="X9" s="4">
+      <c r="X9" s="3">
         <v>76.31</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="3">
         <v>3.11</v>
       </c>
-      <c r="Z9" s="4"/>
-      <c r="AB9" s="4">
+      <c r="Z9" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="AB9" s="3">
         <v>5</v>
       </c>
-      <c r="AC9" s="4">
+      <c r="AC9" s="3">
         <v>64.44</v>
       </c>
-      <c r="AD9" s="4">
+      <c r="AD9" s="3">
         <v>1.22</v>
       </c>
-      <c r="AE9" s="4"/>
+      <c r="AE9" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>5</v>
+      </c>
+      <c r="AH9" s="3">
+        <v>121.15</v>
+      </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C10" s="4">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C10" s="3">
         <v>6</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>2.1</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.21</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="H10" s="4">
+      <c r="F10" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="H10" s="3">
         <v>6</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>2.0299999999999998</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>0.16</v>
       </c>
-      <c r="K10" s="4"/>
-      <c r="M10" s="4">
+      <c r="K10" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="M10" s="3">
         <v>6</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="3">
         <v>7.38</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="3">
         <v>0.39</v>
       </c>
-      <c r="P10" s="4"/>
-      <c r="R10" s="4">
+      <c r="P10" s="3">
+        <v>1.38</v>
+      </c>
+      <c r="R10" s="3">
         <v>6</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10" s="3">
         <v>6.91</v>
       </c>
-      <c r="T10" s="4">
+      <c r="T10" s="3">
         <v>0.26</v>
       </c>
-      <c r="U10" s="4"/>
-      <c r="W10" s="4">
+      <c r="U10" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="W10" s="3">
         <v>6</v>
       </c>
-      <c r="X10" s="4">
+      <c r="X10" s="3">
         <v>79.92</v>
       </c>
-      <c r="Y10" s="4">
+      <c r="Y10" s="3">
         <v>2.46</v>
       </c>
-      <c r="Z10" s="4"/>
-      <c r="AB10" s="4">
+      <c r="Z10" s="3">
+        <v>6.03</v>
+      </c>
+      <c r="AB10" s="3">
         <v>6</v>
       </c>
-      <c r="AC10" s="4">
+      <c r="AC10" s="3">
         <v>70.17</v>
       </c>
-      <c r="AD10" s="4">
+      <c r="AD10" s="3">
         <v>1.1399999999999999</v>
       </c>
-      <c r="AE10" s="4"/>
+      <c r="AE10" s="3">
+        <v>2.88</v>
+      </c>
+      <c r="AG10" s="3">
+        <v>6</v>
+      </c>
+      <c r="AH10" s="3">
+        <v>90.92</v>
+      </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C11" s="4">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C11" s="3">
         <v>7</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>2.34</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>0.22</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="H11" s="4">
+      <c r="F11" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="H11" s="3">
         <v>7</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>2.33</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>0.17</v>
       </c>
-      <c r="K11" s="4"/>
-      <c r="M11" s="4">
+      <c r="K11" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="M11" s="3">
         <v>7</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="3">
         <v>8.0500000000000007</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="3">
         <v>0.41</v>
       </c>
-      <c r="P11" s="4"/>
-      <c r="R11" s="4">
+      <c r="P11" s="3">
+        <v>1.32</v>
+      </c>
+      <c r="R11" s="3">
         <v>7</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="3">
         <v>8.19</v>
       </c>
-      <c r="T11" s="4">
+      <c r="T11" s="3">
         <v>0.27</v>
       </c>
-      <c r="U11" s="4"/>
-      <c r="W11" s="4">
+      <c r="U11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W11" s="3">
         <v>7</v>
       </c>
-      <c r="X11" s="4">
+      <c r="X11" s="3">
         <v>81.040000000000006</v>
       </c>
-      <c r="Y11" s="4">
+      <c r="Y11" s="3">
         <v>2.4700000000000002</v>
       </c>
-      <c r="Z11" s="4"/>
-      <c r="AB11" s="4">
+      <c r="Z11" s="3">
+        <v>5.94</v>
+      </c>
+      <c r="AB11" s="3">
         <v>7</v>
       </c>
-      <c r="AC11" s="4">
+      <c r="AC11" s="3">
         <v>79.17</v>
       </c>
-      <c r="AD11" s="4">
+      <c r="AD11" s="3">
         <v>1.1299999999999999</v>
       </c>
-      <c r="AE11" s="4"/>
+      <c r="AE11" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="AG11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AH11" s="3">
+        <v>90.25</v>
+      </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C12" s="4">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C12" s="3">
         <v>8</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>2.44</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>0.21</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="H12" s="4">
+      <c r="F12" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="H12" s="3">
         <v>8</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>2.41</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>0.19</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="M12" s="4">
+      <c r="K12" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="M12" s="3">
         <v>8</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="3">
         <v>8.9600000000000009</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12" s="3">
         <v>0.38</v>
       </c>
-      <c r="P12" s="4"/>
-      <c r="R12" s="4">
+      <c r="P12" s="3">
+        <v>1.24</v>
+      </c>
+      <c r="R12" s="3">
         <v>8</v>
       </c>
-      <c r="S12" s="4">
+      <c r="S12" s="3">
         <v>8.4</v>
       </c>
-      <c r="T12" s="4">
+      <c r="T12" s="3">
         <v>0.26</v>
       </c>
-      <c r="U12" s="4"/>
-      <c r="W12" s="4">
+      <c r="U12" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="W12" s="3">
         <v>8</v>
       </c>
-      <c r="X12" s="4">
+      <c r="X12" s="3">
         <v>87.74</v>
       </c>
-      <c r="Y12" s="4">
+      <c r="Y12" s="3">
         <v>2.2599999999999998</v>
       </c>
-      <c r="Z12" s="4"/>
-      <c r="AB12" s="4">
+      <c r="Z12" s="3">
+        <v>5.12</v>
+      </c>
+      <c r="AB12" s="3">
         <v>8</v>
       </c>
-      <c r="AC12" s="4">
+      <c r="AC12" s="3">
         <v>88.12</v>
       </c>
-      <c r="AD12" s="4">
+      <c r="AD12" s="3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="AE12" s="4"/>
+      <c r="AE12" s="3">
+        <v>2.68</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>8</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>75.290000000000006</v>
+      </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C13" s="4">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C13" s="3">
+        <v>12</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="H13" s="3">
+        <v>12</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="M13" s="3">
+        <v>12</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="R13" s="3">
+        <v>12</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="W13" s="3">
+        <v>12</v>
+      </c>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3">
+        <v>3.98</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>12</v>
+      </c>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>12</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>62.84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C14" s="3">
         <v>16</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="H13" s="4">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="H14" s="3">
         <v>16</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="M13" s="4">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="M14" s="3">
         <v>16</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="R13" s="4">
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3">
+        <v>1.31</v>
+      </c>
+      <c r="R14" s="3">
         <v>16</v>
       </c>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="W13" s="4">
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W14" s="3">
         <v>16</v>
       </c>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AB13" s="4">
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="AB14" s="3">
         <v>16</v>
       </c>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>16</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>62.8</v>
+      </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C14" s="4">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C15" s="3">
         <v>32</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="H14" s="4">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <v>3.09</v>
+      </c>
+      <c r="H15" s="3">
         <v>32</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="M14" s="4">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3">
+        <v>2.98</v>
+      </c>
+      <c r="M15" s="3">
         <v>32</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="R14" s="4">
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="R15" s="3">
         <v>32</v>
       </c>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="W14" s="4">
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="W15" s="3">
         <v>32</v>
       </c>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AB14" s="4">
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3">
+        <v>5.39</v>
+      </c>
+      <c r="AB15" s="3">
         <v>32</v>
       </c>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3">
+        <v>4.41</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>32</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>45.81</v>
+      </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="C15" s="4">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="C16" s="3">
         <v>64</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="H15" s="4">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>3.05</v>
+      </c>
+      <c r="H16" s="3">
         <v>64</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="M15" s="4">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3">
+        <v>3.01</v>
+      </c>
+      <c r="M16" s="3">
         <v>64</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="R15" s="4">
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3">
+        <v>3.17</v>
+      </c>
+      <c r="R16" s="3">
         <v>64</v>
       </c>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="W15" s="4">
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3">
+        <v>3.12</v>
+      </c>
+      <c r="W16" s="3">
         <v>64</v>
       </c>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AB15" s="4">
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3">
+        <v>4.53</v>
+      </c>
+      <c r="AB16" s="3">
         <v>64</v>
       </c>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3">
+        <v>3.96</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>64</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>29.75</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="W2:Z2"/>
+  <mergeCells count="13">
+    <mergeCell ref="AG2:AH2"/>
     <mergeCell ref="AB2:AE2"/>
     <mergeCell ref="X3:Y3"/>
     <mergeCell ref="AC3:AD3"/>
@@ -1241,6 +1511,11 @@
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="I3:J3"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="W2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor updates to project report
</commit_message>
<xml_diff>
--- a/Project Repport/Comparaison des performances.xlsx
+++ b/Project Repport/Comparaison des performances.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WINDOWS\Téléchargement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\FractalSharp\Project Repport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D035DC5-99EA-45B2-9C2A-F130153F1C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F2D497-BAB8-4993-A95C-3CF75478ED2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -81,10 +81,10 @@
     <t>C++ Linux</t>
   </si>
   <si>
-    <t>wor : -2 2 -1.125 1.125</t>
+    <t>1280*720 : -1.828 -1.64 -0.057 0.049</t>
   </si>
   <si>
-    <t>1280*720 : -1.828 -1.64 -0.057 0.049</t>
+    <t>16000*9000 : -2 2 -1.125 1.125</t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,20 +156,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8704,95 +8697,95 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BV16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AZ2" sqref="AZ2:BC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="8.85546875" style="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="8.85546875" style="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="8.85546875" style="1"/>
-    <col min="19" max="19" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="8.85546875" style="1"/>
-    <col min="24" max="24" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="36" width="8.85546875" style="1"/>
-    <col min="37" max="37" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="41" width="8.85546875" style="1"/>
-    <col min="42" max="42" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="15.5703125" style="1" customWidth="1"/>
-    <col min="44" max="65" width="8.85546875" style="1"/>
-    <col min="66" max="66" width="6.85546875" style="1" customWidth="1"/>
-    <col min="67" max="70" width="8.85546875" style="1" hidden="1" customWidth="1"/>
-    <col min="71" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="63.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="8.88671875" style="1"/>
+    <col min="19" max="19" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="8.88671875" style="1"/>
+    <col min="24" max="24" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="36" width="8.88671875" style="1"/>
+    <col min="37" max="37" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="41" width="8.88671875" style="1"/>
+    <col min="42" max="42" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="15.5546875" style="1" customWidth="1"/>
+    <col min="44" max="65" width="8.88671875" style="1"/>
+    <col min="66" max="66" width="6.88671875" style="1" customWidth="1"/>
+    <col min="67" max="70" width="8.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="71" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="L2" s="5" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="L2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="W2" s="5" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="W2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AE2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AO2" s="5" t="s">
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AE2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AO2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AZ2" s="5" t="s">
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
+      <c r="AZ2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="BA2" s="5"/>
-      <c r="BB2" s="5"/>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="5"/>
-      <c r="BF2" s="5"/>
-      <c r="BG2" s="5"/>
+      <c r="BA2" s="7"/>
+      <c r="BB2" s="7"/>
+      <c r="BC2" s="7"/>
+      <c r="BD2" s="7"/>
+      <c r="BE2" s="7"/>
+      <c r="BF2" s="7"/>
+      <c r="BG2" s="7"/>
       <c r="BI2" s="4"/>
       <c r="BJ2" s="4"/>
       <c r="BK2" s="4"/>
       <c r="BL2" s="4"/>
-      <c r="BS2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="BT2" s="5"/>
-      <c r="BU2" s="5"/>
-      <c r="BV2" s="5"/>
+      <c r="BS2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="BT2" s="7"/>
+      <c r="BU2" s="7"/>
+      <c r="BV2" s="7"/>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.3">
       <c r="D3" s="6" t="s">
         <v>0</v>
       </c>
@@ -8814,12 +8807,12 @@
       <c r="Z3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AE3" s="8"/>
+      <c r="AE3"/>
       <c r="AF3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="AG3" s="6"/>
-      <c r="AH3" s="10" t="s">
+      <c r="AH3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="AP3" s="6" t="s">
@@ -8840,7 +8833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:74" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:74" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
@@ -8877,16 +8870,16 @@
       <c r="Z4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AE4" s="9" t="s">
+      <c r="AE4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AF4" s="10" t="s">
+      <c r="AF4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AG4" s="10" t="s">
+      <c r="AG4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AH4" s="10" t="s">
+      <c r="AH4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AO4" s="2" t="s">
@@ -8920,7 +8913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
@@ -8957,16 +8950,16 @@
       <c r="Z5" s="3">
         <v>2.08</v>
       </c>
-      <c r="AE5" s="10" t="s">
+      <c r="AE5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AF5" s="7">
+      <c r="AF5" s="5">
         <v>2.3199999999999998</v>
       </c>
-      <c r="AG5" s="7">
+      <c r="AG5" s="5">
         <v>0.22</v>
       </c>
-      <c r="AH5" s="7">
+      <c r="AH5" s="5">
         <v>0.8</v>
       </c>
       <c r="AO5" s="3" t="s">
@@ -9000,7 +8993,7 @@
         <v>268.27</v>
       </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C6" s="3">
         <v>2</v>
       </c>
@@ -9037,16 +9030,16 @@
       <c r="Z6" s="3">
         <v>1.67</v>
       </c>
-      <c r="AE6" s="10">
+      <c r="AE6" s="3">
         <v>2</v>
       </c>
-      <c r="AF6" s="7">
+      <c r="AF6" s="5">
         <v>4.45</v>
       </c>
-      <c r="AG6" s="7">
+      <c r="AG6" s="5">
         <v>0.22</v>
       </c>
-      <c r="AH6" s="7">
+      <c r="AH6" s="5">
         <v>1.01</v>
       </c>
       <c r="AO6" s="3">
@@ -9080,7 +9073,7 @@
         <v>133.82</v>
       </c>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C7" s="3">
         <v>3</v>
       </c>
@@ -9117,16 +9110,16 @@
       <c r="Z7" s="3">
         <v>1.91</v>
       </c>
-      <c r="AE7" s="10">
+      <c r="AE7" s="3">
         <v>3</v>
       </c>
-      <c r="AF7" s="7">
+      <c r="AF7" s="5">
         <v>5.15</v>
       </c>
-      <c r="AG7" s="7">
+      <c r="AG7" s="5">
         <v>0.25</v>
       </c>
-      <c r="AH7" s="7">
+      <c r="AH7" s="5">
         <v>1.1399999999999999</v>
       </c>
       <c r="AO7" s="3">
@@ -9160,7 +9153,7 @@
         <v>122.1</v>
       </c>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C8" s="3">
         <v>4</v>
       </c>
@@ -9197,16 +9190,16 @@
       <c r="Z8" s="3">
         <v>1.52</v>
       </c>
-      <c r="AE8" s="10">
+      <c r="AE8" s="3">
         <v>4</v>
       </c>
-      <c r="AF8" s="7">
+      <c r="AF8" s="5">
         <v>5.57</v>
       </c>
-      <c r="AG8" s="7">
+      <c r="AG8" s="5">
         <v>0.23</v>
       </c>
-      <c r="AH8" s="7">
+      <c r="AH8" s="5">
         <v>1.03</v>
       </c>
       <c r="AO8" s="3">
@@ -9240,7 +9233,7 @@
         <v>119.22</v>
       </c>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C9" s="3">
         <v>5</v>
       </c>
@@ -9277,16 +9270,16 @@
       <c r="Z9" s="3">
         <v>1.59</v>
       </c>
-      <c r="AE9" s="10">
+      <c r="AE9" s="3">
         <v>5</v>
       </c>
-      <c r="AF9" s="7">
+      <c r="AF9" s="5">
         <v>6.14</v>
       </c>
-      <c r="AG9" s="7">
+      <c r="AG9" s="5">
         <v>0.24</v>
       </c>
-      <c r="AH9" s="7">
+      <c r="AH9" s="5">
         <v>0.96</v>
       </c>
       <c r="AO9" s="3">
@@ -9320,7 +9313,7 @@
         <v>121.15</v>
       </c>
     </row>
-    <row r="10" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>6</v>
       </c>
@@ -9357,16 +9350,16 @@
       <c r="Z10" s="3">
         <v>1.38</v>
       </c>
-      <c r="AE10" s="10">
+      <c r="AE10" s="3">
         <v>6</v>
       </c>
-      <c r="AF10" s="7">
+      <c r="AF10" s="5">
         <v>6.91</v>
       </c>
-      <c r="AG10" s="7">
+      <c r="AG10" s="5">
         <v>0.26</v>
       </c>
-      <c r="AH10" s="7">
+      <c r="AH10" s="5">
         <v>0.94</v>
       </c>
       <c r="AO10" s="3">
@@ -9400,7 +9393,7 @@
         <v>90.92</v>
       </c>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C11" s="3">
         <v>7</v>
       </c>
@@ -9437,16 +9430,16 @@
       <c r="Z11" s="3">
         <v>1.32</v>
       </c>
-      <c r="AE11" s="10">
+      <c r="AE11" s="3">
         <v>7</v>
       </c>
-      <c r="AF11" s="7">
+      <c r="AF11" s="5">
         <v>8.19</v>
       </c>
-      <c r="AG11" s="7">
+      <c r="AG11" s="5">
         <v>0.27</v>
       </c>
-      <c r="AH11" s="7">
+      <c r="AH11" s="5">
         <v>0.95</v>
       </c>
       <c r="AO11" s="3">
@@ -9480,7 +9473,7 @@
         <v>90.25</v>
       </c>
     </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C12" s="3">
         <v>8</v>
       </c>
@@ -9517,16 +9510,16 @@
       <c r="Z12" s="3">
         <v>1.24</v>
       </c>
-      <c r="AE12" s="10">
+      <c r="AE12" s="3">
         <v>8</v>
       </c>
-      <c r="AF12" s="7">
+      <c r="AF12" s="5">
         <v>8.4</v>
       </c>
-      <c r="AG12" s="7">
+      <c r="AG12" s="5">
         <v>0.26</v>
       </c>
-      <c r="AH12" s="7">
+      <c r="AH12" s="5">
         <v>0.94</v>
       </c>
       <c r="AO12" s="3">
@@ -9560,7 +9553,7 @@
         <v>75.290000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C13" s="3">
         <v>12</v>
       </c>
@@ -9585,12 +9578,12 @@
       <c r="Z13" s="3">
         <v>1.25</v>
       </c>
-      <c r="AE13" s="10">
+      <c r="AE13" s="3">
         <v>16</v>
       </c>
-      <c r="AF13" s="7"/>
-      <c r="AG13" s="7"/>
-      <c r="AH13" s="7">
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
+      <c r="AH13" s="5">
         <v>0.94</v>
       </c>
       <c r="AO13" s="3">
@@ -9616,7 +9609,7 @@
         <v>62.84</v>
       </c>
     </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>16</v>
       </c>
@@ -9641,12 +9634,12 @@
       <c r="Z14" s="3">
         <v>1.31</v>
       </c>
-      <c r="AE14" s="10">
+      <c r="AE14" s="3">
         <v>32</v>
       </c>
-      <c r="AF14" s="7"/>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7">
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5">
         <v>3.1</v>
       </c>
       <c r="AO14" s="3">
@@ -9672,7 +9665,7 @@
         <v>62.8</v>
       </c>
     </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C15" s="3">
         <v>32</v>
       </c>
@@ -9697,12 +9690,12 @@
       <c r="Z15" s="3">
         <v>3.3</v>
       </c>
-      <c r="AE15" s="10">
+      <c r="AE15" s="3">
         <v>64</v>
       </c>
-      <c r="AF15" s="7"/>
-      <c r="AG15" s="7"/>
-      <c r="AH15" s="7">
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="5"/>
+      <c r="AH15" s="5">
         <v>3.12</v>
       </c>
       <c r="AO15" s="3">
@@ -9728,7 +9721,7 @@
         <v>45.81</v>
       </c>
     </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:74" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>64</v>
       </c>

</xml_diff>